<commit_message>
new opcodes was added
</commit_message>
<xml_diff>
--- a/Annotation/WEBVM - OPCODES.xlsx
+++ b/Annotation/WEBVM - OPCODES.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="117">
   <si>
     <t xml:space="preserve">WEBVM – OPCODES</t>
   </si>
@@ -287,6 +287,181 @@
   </si>
   <si>
     <t xml:space="preserve">CPU WILL EMIT TURN OFF SIGNAL FOR ALL COMPONENT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and 0x00 0x00</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAKES LOGICAL “AND” OPERATION BETWEEN REGISTERS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST REGISTER INDICATED.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or 0x00 0x00</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAKES LOGICAL “OR” OPERATION BETWEEN REGISTERS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST REGISTER INDICATED.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">XOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xor 0x00 0x00</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAKES LOGICAL “XOR” OPERATION BETWEEN REGISTERS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST REGISTER INDICATED.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not 0x00 0x00</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAKES LOGICAL “NOT” OPERATION BETWEEN REGISTERS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST REGISTER INDICATED.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nand 0x00 0x00</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAKES LOGICAL “NAND” OPERATION BETWEEN REGISTERS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST REGISTER INDICATED.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nor 0x00 0x02</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAKES LOGICAL “NOR” OPERATION BETWEEN REGISTERS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST REGISTER INDICATED.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">XNOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xnor 0x00 0x03</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAKES LOGICAL “XNOR” OPERATION BETWEEN REGISTERS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. AFTER OPERATION THE VALUE RESULTANT WILL BE STORAGE IN THE LAST REGISTER INDICATED.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">REGISTERS</t>
@@ -316,16 +491,17 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
-    <numFmt numFmtId="165" formatCode="[$R$-416]\ #,##0.00;[RED]\-[$R$-416]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$-407]General"/>
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="[$-407]General"/>
+    <numFmt numFmtId="167" formatCode="[$R$-416]\ #,##0.00;[RED]\-[$R$-416]\ #,##0.00"/>
     <numFmt numFmtId="168" formatCode="[$-409]@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -343,21 +519,29 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFC0C0C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC0C0C0"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="16"/>
       <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -370,12 +554,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9966"/>
-        <bgColor rgb="FFFF99CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF4C1900"/>
         <bgColor rgb="FF333333"/>
       </patternFill>
@@ -384,6 +562,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9966"/>
+        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
     <fill>
@@ -403,62 +587,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair">
-        <color rgb="FF4C1900"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color rgb="FF4C1900"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="hair">
-        <color rgb="FF4C1900"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair">
-        <color rgb="FF4C1900"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF4C1900"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair">
-        <color rgb="FF4C1900"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair">
-        <color rgb="FF4C1900"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -495,6 +623,62 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF4C1900"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair">
+        <color rgb="FF4C1900"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF4C1900"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF4C1900"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF4C1900"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair">
+        <color rgb="FF4C1900"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF4C1900"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -526,45 +710,45 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="167" fontId="5" fillId="4" borderId="9" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="9">
@@ -596,7 +780,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -612,19 +796,19 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Result2" xfId="20"/>
-    <cellStyle name="Background" xfId="21"/>
-    <cellStyle name="Card" xfId="22"/>
-    <cellStyle name="Input" xfId="23"/>
-    <cellStyle name="Card TL" xfId="24"/>
-    <cellStyle name="Card T" xfId="25"/>
-    <cellStyle name="Card TR" xfId="26"/>
-    <cellStyle name="Card L" xfId="27"/>
-    <cellStyle name="Card R" xfId="28"/>
-    <cellStyle name="Card B" xfId="29"/>
-    <cellStyle name="Card BL" xfId="30"/>
-    <cellStyle name="Card BR" xfId="31"/>
-    <cellStyle name="Column Header" xfId="32"/>
+    <cellStyle name="Background" xfId="20"/>
+    <cellStyle name="Card" xfId="21"/>
+    <cellStyle name="Card B" xfId="22"/>
+    <cellStyle name="Card BL" xfId="23"/>
+    <cellStyle name="Card BR" xfId="24"/>
+    <cellStyle name="Card L" xfId="25"/>
+    <cellStyle name="Card R" xfId="26"/>
+    <cellStyle name="Card T" xfId="27"/>
+    <cellStyle name="Card TL" xfId="28"/>
+    <cellStyle name="Card TR" xfId="29"/>
+    <cellStyle name="Column Header" xfId="30"/>
+    <cellStyle name="Input" xfId="31"/>
+    <cellStyle name="Result2" xfId="32"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -694,20 +878,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1140,53 +1324,186 @@
       </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+    <row r="23" customFormat="false" ht="65.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="F23" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="F24" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="33">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -1209,10 +1526,17 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>